<commit_message>
finished simple knapsack voting, still needs proper testing
</commit_message>
<xml_diff>
--- a/threshold_approval.xlsx
+++ b/threshold_approval.xlsx
@@ -473,10 +473,10 @@
         </is>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -498,22 +498,22 @@
         </is>
       </c>
       <c r="B3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
       <c r="E3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -523,7 +523,7 @@
         </is>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -532,13 +532,13 @@
         <v>0</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -548,7 +548,7 @@
         </is>
       </c>
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -560,10 +560,10 @@
         <v>1</v>
       </c>
       <c r="F5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -607,13 +607,13 @@
         <v>0</v>
       </c>
       <c r="E7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
       <c r="G7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -626,16 +626,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -651,16 +651,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
       </c>
       <c r="F9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
@@ -673,7 +673,7 @@
         </is>
       </c>
       <c r="B10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -685,7 +685,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -723,19 +723,19 @@
         </is>
       </c>
       <c r="B12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
       </c>
       <c r="F12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -748,22 +748,22 @@
         </is>
       </c>
       <c r="B13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
       </c>
       <c r="E13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -810,7 +810,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -823,13 +823,13 @@
         </is>
       </c>
       <c r="B16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
       </c>
       <c r="D16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="b">
         <v>1</v>
@@ -848,22 +848,22 @@
         </is>
       </c>
       <c r="B17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -882,13 +882,13 @@
         <v>0</v>
       </c>
       <c r="E18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
       </c>
       <c r="G18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -948,22 +948,22 @@
         </is>
       </c>
       <c r="B21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -973,19 +973,19 @@
         </is>
       </c>
       <c r="B22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Refactored names and file structure.
</commit_message>
<xml_diff>
--- a/threshold_approval.xlsx
+++ b/threshold_approval.xlsx
@@ -1,93 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>project0</t>
-  </si>
-  <si>
-    <t>project1</t>
-  </si>
-  <si>
-    <t>project2</t>
-  </si>
-  <si>
-    <t>project3</t>
-  </si>
-  <si>
-    <t>project4</t>
-  </si>
-  <si>
-    <t>project5</t>
-  </si>
-  <si>
-    <t>voter0</t>
-  </si>
-  <si>
-    <t>voter1</t>
-  </si>
-  <si>
-    <t>voter2</t>
-  </si>
-  <si>
-    <t>voter3</t>
-  </si>
-  <si>
-    <t>voter4</t>
-  </si>
-  <si>
-    <t>voter5</t>
-  </si>
-  <si>
-    <t>voter6</t>
-  </si>
-  <si>
-    <t>voter7</t>
-  </si>
-  <si>
-    <t>voter8</t>
-  </si>
-  <si>
-    <t>voter9</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -102,35 +46,94 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -418,59 +421,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>project0</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>project1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>project2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>project3</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>project4</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>project5</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>voter0</t>
+        </is>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>voter1</t>
+        </is>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -482,7 +507,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -491,9 +516,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>voter2</t>
+        </is>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -502,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -514,15 +541,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>voter3</t>
+        </is>
       </c>
       <c r="B5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -537,32 +566,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>voter4</t>
+        </is>
       </c>
       <c r="B6" t="b">
         <v>1</v>
       </c>
       <c r="C6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
       </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>voter5</t>
+        </is>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -577,15 +610,17 @@
         <v>1</v>
       </c>
       <c r="F7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>voter6</t>
+        </is>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -594,79 +629,85 @@
         <v>1</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>voter7</t>
+        </is>
       </c>
       <c r="B9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>voter8</t>
+        </is>
       </c>
       <c r="B10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
       </c>
       <c r="D10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
       </c>
       <c r="G10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>voter9</t>
+        </is>
       </c>
       <c r="B11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
       </c>
       <c r="D11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -676,6 +717,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>